<commit_message>
Post Home Fix and Rewards fix
</commit_message>
<xml_diff>
--- a/Rumi/LoyaltyProgramModel_v3.xlsx
+++ b/Rumi/LoyaltyProgramModel_v3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\jorge\Loyalty\Rumi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D42CA8E-9E3F-4CC4-9B7E-B2B7102A38D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0025BEDD-F99A-4BF2-9B75-21D7BC0EC349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7534,7 +7534,7 @@
   <dimension ref="A1:T75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W13" sqref="W13"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Post implement fix: /Loyalty/Rumi/BugFixes/RewardsPageSuccessCallbacksNoRefreshFix.md
</commit_message>
<xml_diff>
--- a/Rumi/LoyaltyProgramModel_v3.xlsx
+++ b/Rumi/LoyaltyProgramModel_v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\jorge\Loyalty\Rumi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E792F5B7-61E1-4E70-BBC6-0D8B60A38571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587EF3C4-4290-4C03-9A44-9E2027427D3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Walkthrough" sheetId="1" r:id="rId1"/>
@@ -2201,23 +2201,23 @@
     <xf numFmtId="164" fontId="0" fillId="25" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="34" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="33" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="34" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="43" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="32" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="30" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="32" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="31" fillId="44" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2550,7 +2550,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="213" t="s">
+      <c r="A1" s="210" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="207"/>
@@ -2558,7 +2558,7 @@
       <c r="D1" s="207"/>
     </row>
     <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="209" t="s">
+      <c r="A3" s="214" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="207"/>
@@ -2569,7 +2569,7 @@
       <c r="A4" s="188" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="212" t="s">
+      <c r="B4" s="211" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="207"/>
@@ -2579,7 +2579,7 @@
       <c r="A5" s="189" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="210" t="s">
+      <c r="B5" s="208" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="207"/>
@@ -2589,7 +2589,7 @@
       <c r="A6" s="190" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="206" t="s">
+      <c r="B6" s="209" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="207"/>
@@ -2599,7 +2599,7 @@
       <c r="A7" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="210" t="s">
+      <c r="B7" s="208" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="207"/>
@@ -2609,7 +2609,7 @@
       <c r="A8" s="190" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="206" t="s">
+      <c r="B8" s="209" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="207"/>
@@ -2619,7 +2619,7 @@
       <c r="A9" s="189" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="210" t="s">
+      <c r="B9" s="208" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="207"/>
@@ -2629,7 +2629,7 @@
       <c r="A10" s="190" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="206" t="s">
+      <c r="B10" s="209" t="s">
         <v>15</v>
       </c>
       <c r="C10" s="207"/>
@@ -2639,7 +2639,7 @@
       <c r="A11" s="189" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="210" t="s">
+      <c r="B11" s="208" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="207"/>
@@ -2649,7 +2649,7 @@
       <c r="A12" s="190" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="206" t="s">
+      <c r="B12" s="209" t="s">
         <v>19</v>
       </c>
       <c r="C12" s="207"/>
@@ -2659,14 +2659,14 @@
       <c r="A13" s="189" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="210" t="s">
+      <c r="B13" s="208" t="s">
         <v>21</v>
       </c>
       <c r="C13" s="207"/>
       <c r="D13" s="207"/>
     </row>
     <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="209" t="s">
+      <c r="A15" s="214" t="s">
         <v>22</v>
       </c>
       <c r="B15" s="207"/>
@@ -2680,7 +2680,7 @@
       <c r="B16" s="188" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="212" t="s">
+      <c r="C16" s="211" t="s">
         <v>24</v>
       </c>
       <c r="D16" s="207"/>
@@ -2692,7 +2692,7 @@
       <c r="B17" s="189" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="210" t="s">
+      <c r="C17" s="208" t="s">
         <v>26</v>
       </c>
       <c r="D17" s="207"/>
@@ -2704,10 +2704,10 @@
       <c r="B18" s="190" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="206" t="s">
+      <c r="C18" s="209" t="s">
         <v>296</v>
       </c>
-      <c r="D18" s="211"/>
+      <c r="D18" s="213"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="189" t="s">
@@ -2716,7 +2716,7 @@
       <c r="B19" s="189" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="210" t="s">
+      <c r="C19" s="208" t="s">
         <v>29</v>
       </c>
       <c r="D19" s="207"/>
@@ -2739,10 +2739,10 @@
       <c r="B21" s="190" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="206" t="s">
+      <c r="C21" s="209" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="211"/>
+      <c r="D21" s="213"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="189" t="s">
@@ -2751,7 +2751,7 @@
       <c r="B22" s="189" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="210" t="s">
+      <c r="C22" s="208" t="s">
         <v>33</v>
       </c>
       <c r="D22" s="207"/>
@@ -2774,10 +2774,10 @@
       <c r="B24" s="190" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="206" t="s">
+      <c r="C24" s="209" t="s">
         <v>35</v>
       </c>
-      <c r="D24" s="211"/>
+      <c r="D24" s="213"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="189" t="s">
@@ -2786,7 +2786,7 @@
       <c r="B25" s="189" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="210" t="s">
+      <c r="C25" s="208" t="s">
         <v>37</v>
       </c>
       <c r="D25" s="207"/>
@@ -2798,10 +2798,10 @@
       <c r="B26" s="190" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="206" t="s">
+      <c r="C26" s="209" t="s">
         <v>38</v>
       </c>
-      <c r="D26" s="211"/>
+      <c r="D26" s="213"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="189" t="s">
@@ -2810,7 +2810,7 @@
       <c r="B27" s="189" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="210" t="s">
+      <c r="C27" s="208" t="s">
         <v>40</v>
       </c>
       <c r="D27" s="207"/>
@@ -2822,13 +2822,13 @@
       <c r="B28" s="190" t="s">
         <v>41</v>
       </c>
-      <c r="C28" s="206" t="s">
+      <c r="C28" s="209" t="s">
         <v>42</v>
       </c>
-      <c r="D28" s="211"/>
+      <c r="D28" s="213"/>
     </row>
     <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="209" t="s">
+      <c r="A31" s="214" t="s">
         <v>43</v>
       </c>
       <c r="B31" s="207"/>
@@ -2842,7 +2842,7 @@
       <c r="B32" s="188" t="s">
         <v>23</v>
       </c>
-      <c r="C32" s="212" t="s">
+      <c r="C32" s="211" t="s">
         <v>44</v>
       </c>
       <c r="D32" s="207"/>
@@ -2854,7 +2854,7 @@
       <c r="B33" s="189" t="s">
         <v>304</v>
       </c>
-      <c r="C33" s="210" t="s">
+      <c r="C33" s="208" t="s">
         <v>184</v>
       </c>
       <c r="D33" s="207"/>
@@ -2866,10 +2866,10 @@
       <c r="B34" s="190" t="s">
         <v>305</v>
       </c>
-      <c r="C34" s="206" t="s">
+      <c r="C34" s="209" t="s">
         <v>307</v>
       </c>
-      <c r="D34" s="211"/>
+      <c r="D34" s="213"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="189" t="s">
@@ -2878,7 +2878,7 @@
       <c r="B35" s="189" t="s">
         <v>297</v>
       </c>
-      <c r="C35" s="210" t="s">
+      <c r="C35" s="208" t="s">
         <v>45</v>
       </c>
       <c r="D35" s="207"/>
@@ -2890,13 +2890,13 @@
       <c r="B36" s="190" t="s">
         <v>298</v>
       </c>
-      <c r="C36" s="206" t="s">
+      <c r="C36" s="209" t="s">
         <v>46</v>
       </c>
-      <c r="D36" s="211"/>
+      <c r="D36" s="213"/>
     </row>
     <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="214" t="s">
+      <c r="A39" s="212" t="s">
         <v>47</v>
       </c>
       <c r="B39" s="207"/>
@@ -2904,7 +2904,7 @@
       <c r="D39" s="207"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="208" t="s">
+      <c r="A40" s="206" t="s">
         <v>48</v>
       </c>
       <c r="B40" s="207"/>
@@ -2912,13 +2912,13 @@
       <c r="D40" s="207"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="208"/>
+      <c r="A41" s="206"/>
       <c r="B41" s="207"/>
       <c r="C41" s="207"/>
       <c r="D41" s="207"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="208" t="s">
+      <c r="A42" s="206" t="s">
         <v>49</v>
       </c>
       <c r="B42" s="207"/>
@@ -2926,7 +2926,7 @@
       <c r="D42" s="207"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="208" t="s">
+      <c r="A43" s="206" t="s">
         <v>50</v>
       </c>
       <c r="B43" s="207"/>
@@ -2934,7 +2934,7 @@
       <c r="D43" s="207"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="208" t="s">
+      <c r="A44" s="206" t="s">
         <v>51</v>
       </c>
       <c r="B44" s="207"/>
@@ -2942,13 +2942,13 @@
       <c r="D44" s="207"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="208"/>
+      <c r="A45" s="206"/>
       <c r="B45" s="207"/>
       <c r="C45" s="207"/>
       <c r="D45" s="207"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="208" t="s">
+      <c r="A46" s="206" t="s">
         <v>52</v>
       </c>
       <c r="B46" s="207"/>
@@ -2956,7 +2956,7 @@
       <c r="D46" s="207"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="208" t="s">
+      <c r="A47" s="206" t="s">
         <v>53</v>
       </c>
       <c r="B47" s="207"/>
@@ -2964,7 +2964,7 @@
       <c r="D47" s="207"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="208" t="s">
+      <c r="A48" s="206" t="s">
         <v>54</v>
       </c>
       <c r="B48" s="207"/>
@@ -2973,6 +2973,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="A47:D47"/>
+    <mergeCell ref="A44:D44"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="B12:D12"/>
     <mergeCell ref="A48:D48"/>
     <mergeCell ref="C35:D35"/>
     <mergeCell ref="B6:D6"/>
@@ -2989,30 +3013,6 @@
     <mergeCell ref="A39:D39"/>
     <mergeCell ref="C36:D36"/>
     <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A47:D47"/>
-    <mergeCell ref="A44:D44"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="A41:D41"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="A40:D40"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="B9:D9"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -6169,8 +6169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6465,14 +6465,14 @@
         <v>0.1</v>
       </c>
       <c r="H12" s="40">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I12" s="40" t="s">
         <v>151</v>
       </c>
       <c r="J12" s="46">
         <f>IF(D12="Weekly",4,1)*IF(F12="Gift Card",G12,IF(F12="Spark Ads",G12,IF(F12="Commission Boost",G12*(INDEX('VIP Levels'!$E$5:$E$9,MATCH(A12,'VIP Levels'!$B$5:$B$9,0))*Inputs!$B$14/30*H12)*Revenue!$B$7,IF(F12="Discount",G12*(INDEX('VIP Levels'!$E$5:$E$9,MATCH(A12,'VIP Levels'!$B$5:$B$9,0))*Inputs!$B$14/30*H12)*Inputs!$B$12,0))))</f>
-        <v>30.934843333333337</v>
+        <v>22.09631666666667</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -7117,47 +7117,47 @@
       </c>
       <c r="C9" s="8">
         <f t="shared" si="3"/>
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D9" s="8">
         <f t="shared" si="3"/>
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="E9" s="8">
         <f t="shared" si="3"/>
-        <v>1407</v>
+        <v>1405</v>
       </c>
       <c r="F9" s="8">
         <f t="shared" si="3"/>
-        <v>1969</v>
+        <v>1965</v>
       </c>
       <c r="G9" s="8">
         <f t="shared" si="3"/>
-        <v>2597</v>
+        <v>2591</v>
       </c>
       <c r="H9" s="8">
         <f t="shared" si="3"/>
-        <v>3377</v>
+        <v>3369</v>
       </c>
       <c r="I9" s="8">
         <f t="shared" si="3"/>
-        <v>4255</v>
+        <v>4245</v>
       </c>
       <c r="J9" s="8">
         <f t="shared" si="3"/>
-        <v>5154</v>
+        <v>5142</v>
       </c>
       <c r="K9" s="8">
         <f t="shared" si="3"/>
-        <v>6178</v>
+        <v>6163</v>
       </c>
       <c r="L9" s="8">
         <f t="shared" si="3"/>
-        <v>7301</v>
+        <v>7282</v>
       </c>
       <c r="M9" s="8">
         <f t="shared" si="3"/>
-        <v>8533</v>
+        <v>8511</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -7223,47 +7223,47 @@
       </c>
       <c r="C11" s="8">
         <f>ROUND(C19*'VIP Levels'!$B$16*'VIP Levels'!$E$5*(Inputs!$B$14-1)*('VIP Levels'!$D$16/30)+C20*'VIP Levels'!$B$17*'VIP Levels'!$E$6*(Inputs!$B$14-1)*('VIP Levels'!$D$17/30)+C21*'VIP Levels'!$B$18*'VIP Levels'!$E$7*(Inputs!$B$14-1)*('VIP Levels'!$D$18/30)+C22*'VIP Levels'!$B$19*'VIP Levels'!$E$8*(Inputs!$B$14-1)*('VIP Levels'!$D$19/30)+C23*'VIP Levels'!$B$20*'VIP Levels'!$E$9*(Inputs!$B$14-1)*('VIP Levels'!$D$20/30)+C19*'VIP Levels'!$B$24*'VIP Levels'!$E$5*(Inputs!$B$14-1)*('VIP Levels'!$D$24/30)+C20*'VIP Levels'!$B$25*'VIP Levels'!$E$6*(Inputs!$B$14-1)*('VIP Levels'!$D$25/30)+C21*'VIP Levels'!$B$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*('VIP Levels'!$D$26/30)+C22*'VIP Levels'!$B$27*'VIP Levels'!$E$8*(Inputs!$B$14-1)*('VIP Levels'!$D$27/30)+C23*'VIP Levels'!$B$28*'VIP Levels'!$E$9*(Inputs!$B$14-1)*('VIP Levels'!$D$28/30)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26="One-time")*C19*Missions!$E$5:$E$26*'VIP Levels'!$E$5*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*C13*Missions!$E$5:$E$26*'VIP Levels'!$E$5*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26="One-time")*C20*Missions!$E$5:$E$26*'VIP Levels'!$E$6*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*C14*Missions!$E$5:$E$26*'VIP Levels'!$E$6*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26="One-time")*C21*Missions!$E$5:$E$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*C15*Missions!$E$5:$E$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26="One-time")*C22*Missions!$E$5:$E$26*'VIP Levels'!$E$8*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*C16*Missions!$E$5:$E$26*'VIP Levels'!$E$8*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26="One-time")*C23*Missions!$E$5:$E$26*'VIP Levels'!$E$9*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*C17*Missions!$E$5:$E$26*'VIP Levels'!$E$9*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26="One-time")*C19*Missions!$E$5:$E$26*'VIP Levels'!$E$5*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*C13*Missions!$E$5:$E$26*'VIP Levels'!$E$5*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26="One-time")*C20*Missions!$E$5:$E$26*'VIP Levels'!$E$6*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*C14*Missions!$E$5:$E$26*'VIP Levels'!$E$6*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26="One-time")*C21*Missions!$E$5:$E$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*C15*Missions!$E$5:$E$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26="One-time")*C22*Missions!$E$5:$E$26*'VIP Levels'!$E$8*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*C16*Missions!$E$5:$E$26*'VIP Levels'!$E$8*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26="One-time")*C23*Missions!$E$5:$E$26*'VIP Levels'!$E$9*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*C17*Missions!$E$5:$E$26*'VIP Levels'!$E$9*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30)),0)</f>
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D11" s="8">
         <f>ROUND(D19*'VIP Levels'!$B$16*'VIP Levels'!$E$5*(Inputs!$B$14-1)*('VIP Levels'!$D$16/30)+D20*'VIP Levels'!$B$17*'VIP Levels'!$E$6*(Inputs!$B$14-1)*('VIP Levels'!$D$17/30)+D21*'VIP Levels'!$B$18*'VIP Levels'!$E$7*(Inputs!$B$14-1)*('VIP Levels'!$D$18/30)+D22*'VIP Levels'!$B$19*'VIP Levels'!$E$8*(Inputs!$B$14-1)*('VIP Levels'!$D$19/30)+D23*'VIP Levels'!$B$20*'VIP Levels'!$E$9*(Inputs!$B$14-1)*('VIP Levels'!$D$20/30)+D19*'VIP Levels'!$B$24*'VIP Levels'!$E$5*(Inputs!$B$14-1)*('VIP Levels'!$D$24/30)+D20*'VIP Levels'!$B$25*'VIP Levels'!$E$6*(Inputs!$B$14-1)*('VIP Levels'!$D$25/30)+D21*'VIP Levels'!$B$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*('VIP Levels'!$D$26/30)+D22*'VIP Levels'!$B$27*'VIP Levels'!$E$8*(Inputs!$B$14-1)*('VIP Levels'!$D$27/30)+D23*'VIP Levels'!$B$28*'VIP Levels'!$E$9*(Inputs!$B$14-1)*('VIP Levels'!$D$28/30)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26="One-time")*D19*Missions!$E$5:$E$26*'VIP Levels'!$E$5*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*D13*Missions!$E$5:$E$26*'VIP Levels'!$E$5*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26="One-time")*D20*Missions!$E$5:$E$26*'VIP Levels'!$E$6*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*D14*Missions!$E$5:$E$26*'VIP Levels'!$E$6*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26="One-time")*D21*Missions!$E$5:$E$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*D15*Missions!$E$5:$E$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26="One-time")*D22*Missions!$E$5:$E$26*'VIP Levels'!$E$8*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*D16*Missions!$E$5:$E$26*'VIP Levels'!$E$8*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26="One-time")*D23*Missions!$E$5:$E$26*'VIP Levels'!$E$9*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*D17*Missions!$E$5:$E$26*'VIP Levels'!$E$9*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26="One-time")*D19*Missions!$E$5:$E$26*'VIP Levels'!$E$5*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*D13*Missions!$E$5:$E$26*'VIP Levels'!$E$5*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26="One-time")*D20*Missions!$E$5:$E$26*'VIP Levels'!$E$6*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*D14*Missions!$E$5:$E$26*'VIP Levels'!$E$6*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26="One-time")*D21*Missions!$E$5:$E$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*D15*Missions!$E$5:$E$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26="One-time")*D22*Missions!$E$5:$E$26*'VIP Levels'!$E$8*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*D16*Missions!$E$5:$E$26*'VIP Levels'!$E$8*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26="One-time")*D23*Missions!$E$5:$E$26*'VIP Levels'!$E$9*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*D17*Missions!$E$5:$E$26*'VIP Levels'!$E$9*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30)),0)</f>
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E11" s="8">
         <f>ROUND(E19*'VIP Levels'!$B$16*'VIP Levels'!$E$5*(Inputs!$B$14-1)*('VIP Levels'!$D$16/30)+E20*'VIP Levels'!$B$17*'VIP Levels'!$E$6*(Inputs!$B$14-1)*('VIP Levels'!$D$17/30)+E21*'VIP Levels'!$B$18*'VIP Levels'!$E$7*(Inputs!$B$14-1)*('VIP Levels'!$D$18/30)+E22*'VIP Levels'!$B$19*'VIP Levels'!$E$8*(Inputs!$B$14-1)*('VIP Levels'!$D$19/30)+E23*'VIP Levels'!$B$20*'VIP Levels'!$E$9*(Inputs!$B$14-1)*('VIP Levels'!$D$20/30)+E19*'VIP Levels'!$B$24*'VIP Levels'!$E$5*(Inputs!$B$14-1)*('VIP Levels'!$D$24/30)+E20*'VIP Levels'!$B$25*'VIP Levels'!$E$6*(Inputs!$B$14-1)*('VIP Levels'!$D$25/30)+E21*'VIP Levels'!$B$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*('VIP Levels'!$D$26/30)+E22*'VIP Levels'!$B$27*'VIP Levels'!$E$8*(Inputs!$B$14-1)*('VIP Levels'!$D$27/30)+E23*'VIP Levels'!$B$28*'VIP Levels'!$E$9*(Inputs!$B$14-1)*('VIP Levels'!$D$28/30)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26="One-time")*E19*Missions!$E$5:$E$26*'VIP Levels'!$E$5*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*E13*Missions!$E$5:$E$26*'VIP Levels'!$E$5*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26="One-time")*E20*Missions!$E$5:$E$26*'VIP Levels'!$E$6*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*E14*Missions!$E$5:$E$26*'VIP Levels'!$E$6*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26="One-time")*E21*Missions!$E$5:$E$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*E15*Missions!$E$5:$E$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26="One-time")*E22*Missions!$E$5:$E$26*'VIP Levels'!$E$8*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*E16*Missions!$E$5:$E$26*'VIP Levels'!$E$8*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26="One-time")*E23*Missions!$E$5:$E$26*'VIP Levels'!$E$9*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*E17*Missions!$E$5:$E$26*'VIP Levels'!$E$9*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26="One-time")*E19*Missions!$E$5:$E$26*'VIP Levels'!$E$5*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*E13*Missions!$E$5:$E$26*'VIP Levels'!$E$5*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26="One-time")*E20*Missions!$E$5:$E$26*'VIP Levels'!$E$6*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*E14*Missions!$E$5:$E$26*'VIP Levels'!$E$6*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26="One-time")*E21*Missions!$E$5:$E$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*E15*Missions!$E$5:$E$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26="One-time")*E22*Missions!$E$5:$E$26*'VIP Levels'!$E$8*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*E16*Missions!$E$5:$E$26*'VIP Levels'!$E$8*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26="One-time")*E23*Missions!$E$5:$E$26*'VIP Levels'!$E$9*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*E17*Missions!$E$5:$E$26*'VIP Levels'!$E$9*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30)),0)</f>
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F11" s="8">
         <f>ROUND(F19*'VIP Levels'!$B$16*'VIP Levels'!$E$5*(Inputs!$B$14-1)*('VIP Levels'!$D$16/30)+F20*'VIP Levels'!$B$17*'VIP Levels'!$E$6*(Inputs!$B$14-1)*('VIP Levels'!$D$17/30)+F21*'VIP Levels'!$B$18*'VIP Levels'!$E$7*(Inputs!$B$14-1)*('VIP Levels'!$D$18/30)+F22*'VIP Levels'!$B$19*'VIP Levels'!$E$8*(Inputs!$B$14-1)*('VIP Levels'!$D$19/30)+F23*'VIP Levels'!$B$20*'VIP Levels'!$E$9*(Inputs!$B$14-1)*('VIP Levels'!$D$20/30)+F19*'VIP Levels'!$B$24*'VIP Levels'!$E$5*(Inputs!$B$14-1)*('VIP Levels'!$D$24/30)+F20*'VIP Levels'!$B$25*'VIP Levels'!$E$6*(Inputs!$B$14-1)*('VIP Levels'!$D$25/30)+F21*'VIP Levels'!$B$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*('VIP Levels'!$D$26/30)+F22*'VIP Levels'!$B$27*'VIP Levels'!$E$8*(Inputs!$B$14-1)*('VIP Levels'!$D$27/30)+F23*'VIP Levels'!$B$28*'VIP Levels'!$E$9*(Inputs!$B$14-1)*('VIP Levels'!$D$28/30)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26="One-time")*F19*Missions!$E$5:$E$26*'VIP Levels'!$E$5*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*F13*Missions!$E$5:$E$26*'VIP Levels'!$E$5*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26="One-time")*F20*Missions!$E$5:$E$26*'VIP Levels'!$E$6*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*F14*Missions!$E$5:$E$26*'VIP Levels'!$E$6*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26="One-time")*F21*Missions!$E$5:$E$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*F15*Missions!$E$5:$E$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26="One-time")*F22*Missions!$E$5:$E$26*'VIP Levels'!$E$8*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*F16*Missions!$E$5:$E$26*'VIP Levels'!$E$8*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26="One-time")*F23*Missions!$E$5:$E$26*'VIP Levels'!$E$9*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*F17*Missions!$E$5:$E$26*'VIP Levels'!$E$9*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26="One-time")*F19*Missions!$E$5:$E$26*'VIP Levels'!$E$5*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*F13*Missions!$E$5:$E$26*'VIP Levels'!$E$5*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26="One-time")*F20*Missions!$E$5:$E$26*'VIP Levels'!$E$6*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*F14*Missions!$E$5:$E$26*'VIP Levels'!$E$6*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26="One-time")*F21*Missions!$E$5:$E$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*F15*Missions!$E$5:$E$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26="One-time")*F22*Missions!$E$5:$E$26*'VIP Levels'!$E$8*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*F16*Missions!$E$5:$E$26*'VIP Levels'!$E$8*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26="One-time")*F23*Missions!$E$5:$E$26*'VIP Levels'!$E$9*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*F17*Missions!$E$5:$E$26*'VIP Levels'!$E$9*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30)),0)</f>
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="G11" s="8">
         <f>ROUND(G19*'VIP Levels'!$B$16*'VIP Levels'!$E$5*(Inputs!$B$14-1)*('VIP Levels'!$D$16/30)+G20*'VIP Levels'!$B$17*'VIP Levels'!$E$6*(Inputs!$B$14-1)*('VIP Levels'!$D$17/30)+G21*'VIP Levels'!$B$18*'VIP Levels'!$E$7*(Inputs!$B$14-1)*('VIP Levels'!$D$18/30)+G22*'VIP Levels'!$B$19*'VIP Levels'!$E$8*(Inputs!$B$14-1)*('VIP Levels'!$D$19/30)+G23*'VIP Levels'!$B$20*'VIP Levels'!$E$9*(Inputs!$B$14-1)*('VIP Levels'!$D$20/30)+G19*'VIP Levels'!$B$24*'VIP Levels'!$E$5*(Inputs!$B$14-1)*('VIP Levels'!$D$24/30)+G20*'VIP Levels'!$B$25*'VIP Levels'!$E$6*(Inputs!$B$14-1)*('VIP Levels'!$D$25/30)+G21*'VIP Levels'!$B$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*('VIP Levels'!$D$26/30)+G22*'VIP Levels'!$B$27*'VIP Levels'!$E$8*(Inputs!$B$14-1)*('VIP Levels'!$D$27/30)+G23*'VIP Levels'!$B$28*'VIP Levels'!$E$9*(Inputs!$B$14-1)*('VIP Levels'!$D$28/30)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26="One-time")*G19*Missions!$E$5:$E$26*'VIP Levels'!$E$5*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*G13*Missions!$E$5:$E$26*'VIP Levels'!$E$5*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26="One-time")*G20*Missions!$E$5:$E$26*'VIP Levels'!$E$6*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*G14*Missions!$E$5:$E$26*'VIP Levels'!$E$6*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26="One-time")*G21*Missions!$E$5:$E$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*G15*Missions!$E$5:$E$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26="One-time")*G22*Missions!$E$5:$E$26*'VIP Levels'!$E$8*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*G16*Missions!$E$5:$E$26*'VIP Levels'!$E$8*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26="One-time")*G23*Missions!$E$5:$E$26*'VIP Levels'!$E$9*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*G17*Missions!$E$5:$E$26*'VIP Levels'!$E$9*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26="One-time")*G19*Missions!$E$5:$E$26*'VIP Levels'!$E$5*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*G13*Missions!$E$5:$E$26*'VIP Levels'!$E$5*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26="One-time")*G20*Missions!$E$5:$E$26*'VIP Levels'!$E$6*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*G14*Missions!$E$5:$E$26*'VIP Levels'!$E$6*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26="One-time")*G21*Missions!$E$5:$E$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*G15*Missions!$E$5:$E$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26="One-time")*G22*Missions!$E$5:$E$26*'VIP Levels'!$E$8*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*G16*Missions!$E$5:$E$26*'VIP Levels'!$E$8*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26="One-time")*G23*Missions!$E$5:$E$26*'VIP Levels'!$E$9*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*G17*Missions!$E$5:$E$26*'VIP Levels'!$E$9*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30)),0)</f>
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="H11" s="8">
         <f>ROUND(H19*'VIP Levels'!$B$16*'VIP Levels'!$E$5*(Inputs!$B$14-1)*('VIP Levels'!$D$16/30)+H20*'VIP Levels'!$B$17*'VIP Levels'!$E$6*(Inputs!$B$14-1)*('VIP Levels'!$D$17/30)+H21*'VIP Levels'!$B$18*'VIP Levels'!$E$7*(Inputs!$B$14-1)*('VIP Levels'!$D$18/30)+H22*'VIP Levels'!$B$19*'VIP Levels'!$E$8*(Inputs!$B$14-1)*('VIP Levels'!$D$19/30)+H23*'VIP Levels'!$B$20*'VIP Levels'!$E$9*(Inputs!$B$14-1)*('VIP Levels'!$D$20/30)+H19*'VIP Levels'!$B$24*'VIP Levels'!$E$5*(Inputs!$B$14-1)*('VIP Levels'!$D$24/30)+H20*'VIP Levels'!$B$25*'VIP Levels'!$E$6*(Inputs!$B$14-1)*('VIP Levels'!$D$25/30)+H21*'VIP Levels'!$B$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*('VIP Levels'!$D$26/30)+H22*'VIP Levels'!$B$27*'VIP Levels'!$E$8*(Inputs!$B$14-1)*('VIP Levels'!$D$27/30)+H23*'VIP Levels'!$B$28*'VIP Levels'!$E$9*(Inputs!$B$14-1)*('VIP Levels'!$D$28/30)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26="One-time")*H19*Missions!$E$5:$E$26*'VIP Levels'!$E$5*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*H13*Missions!$E$5:$E$26*'VIP Levels'!$E$5*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26="One-time")*H20*Missions!$E$5:$E$26*'VIP Levels'!$E$6*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*H14*Missions!$E$5:$E$26*'VIP Levels'!$E$6*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26="One-time")*H21*Missions!$E$5:$E$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*H15*Missions!$E$5:$E$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26="One-time")*H22*Missions!$E$5:$E$26*'VIP Levels'!$E$8*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*H16*Missions!$E$5:$E$26*'VIP Levels'!$E$8*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26="One-time")*H23*Missions!$E$5:$E$26*'VIP Levels'!$E$9*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*H17*Missions!$E$5:$E$26*'VIP Levels'!$E$9*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26="One-time")*H19*Missions!$E$5:$E$26*'VIP Levels'!$E$5*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*H13*Missions!$E$5:$E$26*'VIP Levels'!$E$5*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26="One-time")*H20*Missions!$E$5:$E$26*'VIP Levels'!$E$6*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*H14*Missions!$E$5:$E$26*'VIP Levels'!$E$6*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26="One-time")*H21*Missions!$E$5:$E$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*H15*Missions!$E$5:$E$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26="One-time")*H22*Missions!$E$5:$E$26*'VIP Levels'!$E$8*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*H16*Missions!$E$5:$E$26*'VIP Levels'!$E$8*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26="One-time")*H23*Missions!$E$5:$E$26*'VIP Levels'!$E$9*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*H17*Missions!$E$5:$E$26*'VIP Levels'!$E$9*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30)),0)</f>
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="I11" s="8">
         <f>ROUND(I19*'VIP Levels'!$B$16*'VIP Levels'!$E$5*(Inputs!$B$14-1)*('VIP Levels'!$D$16/30)+I20*'VIP Levels'!$B$17*'VIP Levels'!$E$6*(Inputs!$B$14-1)*('VIP Levels'!$D$17/30)+I21*'VIP Levels'!$B$18*'VIP Levels'!$E$7*(Inputs!$B$14-1)*('VIP Levels'!$D$18/30)+I22*'VIP Levels'!$B$19*'VIP Levels'!$E$8*(Inputs!$B$14-1)*('VIP Levels'!$D$19/30)+I23*'VIP Levels'!$B$20*'VIP Levels'!$E$9*(Inputs!$B$14-1)*('VIP Levels'!$D$20/30)+I19*'VIP Levels'!$B$24*'VIP Levels'!$E$5*(Inputs!$B$14-1)*('VIP Levels'!$D$24/30)+I20*'VIP Levels'!$B$25*'VIP Levels'!$E$6*(Inputs!$B$14-1)*('VIP Levels'!$D$25/30)+I21*'VIP Levels'!$B$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*('VIP Levels'!$D$26/30)+I22*'VIP Levels'!$B$27*'VIP Levels'!$E$8*(Inputs!$B$14-1)*('VIP Levels'!$D$27/30)+I23*'VIP Levels'!$B$28*'VIP Levels'!$E$9*(Inputs!$B$14-1)*('VIP Levels'!$D$28/30)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26="One-time")*I19*Missions!$E$5:$E$26*'VIP Levels'!$E$5*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*I13*Missions!$E$5:$E$26*'VIP Levels'!$E$5*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26="One-time")*I20*Missions!$E$5:$E$26*'VIP Levels'!$E$6*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*I14*Missions!$E$5:$E$26*'VIP Levels'!$E$6*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26="One-time")*I21*Missions!$E$5:$E$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*I15*Missions!$E$5:$E$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26="One-time")*I22*Missions!$E$5:$E$26*'VIP Levels'!$E$8*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*I16*Missions!$E$5:$E$26*'VIP Levels'!$E$8*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26="One-time")*I23*Missions!$E$5:$E$26*'VIP Levels'!$E$9*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*I17*Missions!$E$5:$E$26*'VIP Levels'!$E$9*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26="One-time")*I19*Missions!$E$5:$E$26*'VIP Levels'!$E$5*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*I13*Missions!$E$5:$E$26*'VIP Levels'!$E$5*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26="One-time")*I20*Missions!$E$5:$E$26*'VIP Levels'!$E$6*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*I14*Missions!$E$5:$E$26*'VIP Levels'!$E$6*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26="One-time")*I21*Missions!$E$5:$E$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*I15*Missions!$E$5:$E$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26="One-time")*I22*Missions!$E$5:$E$26*'VIP Levels'!$E$8*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*I16*Missions!$E$5:$E$26*'VIP Levels'!$E$8*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26="One-time")*I23*Missions!$E$5:$E$26*'VIP Levels'!$E$9*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*I17*Missions!$E$5:$E$26*'VIP Levels'!$E$9*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30)),0)</f>
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="J11" s="8">
         <f>ROUND(J19*'VIP Levels'!$B$16*'VIP Levels'!$E$5*(Inputs!$B$14-1)*('VIP Levels'!$D$16/30)+J20*'VIP Levels'!$B$17*'VIP Levels'!$E$6*(Inputs!$B$14-1)*('VIP Levels'!$D$17/30)+J21*'VIP Levels'!$B$18*'VIP Levels'!$E$7*(Inputs!$B$14-1)*('VIP Levels'!$D$18/30)+J22*'VIP Levels'!$B$19*'VIP Levels'!$E$8*(Inputs!$B$14-1)*('VIP Levels'!$D$19/30)+J23*'VIP Levels'!$B$20*'VIP Levels'!$E$9*(Inputs!$B$14-1)*('VIP Levels'!$D$20/30)+J19*'VIP Levels'!$B$24*'VIP Levels'!$E$5*(Inputs!$B$14-1)*('VIP Levels'!$D$24/30)+J20*'VIP Levels'!$B$25*'VIP Levels'!$E$6*(Inputs!$B$14-1)*('VIP Levels'!$D$25/30)+J21*'VIP Levels'!$B$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*('VIP Levels'!$D$26/30)+J22*'VIP Levels'!$B$27*'VIP Levels'!$E$8*(Inputs!$B$14-1)*('VIP Levels'!$D$27/30)+J23*'VIP Levels'!$B$28*'VIP Levels'!$E$9*(Inputs!$B$14-1)*('VIP Levels'!$D$28/30)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26="One-time")*J19*Missions!$E$5:$E$26*'VIP Levels'!$E$5*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*J13*Missions!$E$5:$E$26*'VIP Levels'!$E$5*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26="One-time")*J20*Missions!$E$5:$E$26*'VIP Levels'!$E$6*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*J14*Missions!$E$5:$E$26*'VIP Levels'!$E$6*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26="One-time")*J21*Missions!$E$5:$E$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*J15*Missions!$E$5:$E$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26="One-time")*J22*Missions!$E$5:$E$26*'VIP Levels'!$E$8*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*J16*Missions!$E$5:$E$26*'VIP Levels'!$E$8*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26="One-time")*J23*Missions!$E$5:$E$26*'VIP Levels'!$E$9*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*J17*Missions!$E$5:$E$26*'VIP Levels'!$E$9*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26="One-time")*J19*Missions!$E$5:$E$26*'VIP Levels'!$E$5*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*J13*Missions!$E$5:$E$26*'VIP Levels'!$E$5*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26="One-time")*J20*Missions!$E$5:$E$26*'VIP Levels'!$E$6*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*J14*Missions!$E$5:$E$26*'VIP Levels'!$E$6*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26="One-time")*J21*Missions!$E$5:$E$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*J15*Missions!$E$5:$E$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26="One-time")*J22*Missions!$E$5:$E$26*'VIP Levels'!$E$8*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*J16*Missions!$E$5:$E$26*'VIP Levels'!$E$8*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26="One-time")*J23*Missions!$E$5:$E$26*'VIP Levels'!$E$9*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*J17*Missions!$E$5:$E$26*'VIP Levels'!$E$9*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30)),0)</f>
-        <v>324</v>
+        <v>312</v>
       </c>
       <c r="K11" s="8">
         <f>ROUND(K19*'VIP Levels'!$B$16*'VIP Levels'!$E$5*(Inputs!$B$14-1)*('VIP Levels'!$D$16/30)+K20*'VIP Levels'!$B$17*'VIP Levels'!$E$6*(Inputs!$B$14-1)*('VIP Levels'!$D$17/30)+K21*'VIP Levels'!$B$18*'VIP Levels'!$E$7*(Inputs!$B$14-1)*('VIP Levels'!$D$18/30)+K22*'VIP Levels'!$B$19*'VIP Levels'!$E$8*(Inputs!$B$14-1)*('VIP Levels'!$D$19/30)+K23*'VIP Levels'!$B$20*'VIP Levels'!$E$9*(Inputs!$B$14-1)*('VIP Levels'!$D$20/30)+K19*'VIP Levels'!$B$24*'VIP Levels'!$E$5*(Inputs!$B$14-1)*('VIP Levels'!$D$24/30)+K20*'VIP Levels'!$B$25*'VIP Levels'!$E$6*(Inputs!$B$14-1)*('VIP Levels'!$D$25/30)+K21*'VIP Levels'!$B$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*('VIP Levels'!$D$26/30)+K22*'VIP Levels'!$B$27*'VIP Levels'!$E$8*(Inputs!$B$14-1)*('VIP Levels'!$D$27/30)+K23*'VIP Levels'!$B$28*'VIP Levels'!$E$9*(Inputs!$B$14-1)*('VIP Levels'!$D$28/30)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26="One-time")*K19*Missions!$E$5:$E$26*'VIP Levels'!$E$5*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*K13*Missions!$E$5:$E$26*'VIP Levels'!$E$5*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26="One-time")*K20*Missions!$E$5:$E$26*'VIP Levels'!$E$6*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*K14*Missions!$E$5:$E$26*'VIP Levels'!$E$6*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26="One-time")*K21*Missions!$E$5:$E$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*K15*Missions!$E$5:$E$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26="One-time")*K22*Missions!$E$5:$E$26*'VIP Levels'!$E$8*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*K16*Missions!$E$5:$E$26*'VIP Levels'!$E$8*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26="One-time")*K23*Missions!$E$5:$E$26*'VIP Levels'!$E$9*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*K17*Missions!$E$5:$E$26*'VIP Levels'!$E$9*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26="One-time")*K19*Missions!$E$5:$E$26*'VIP Levels'!$E$5*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*K13*Missions!$E$5:$E$26*'VIP Levels'!$E$5*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26="One-time")*K20*Missions!$E$5:$E$26*'VIP Levels'!$E$6*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*K14*Missions!$E$5:$E$26*'VIP Levels'!$E$6*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26="One-time")*K21*Missions!$E$5:$E$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*K15*Missions!$E$5:$E$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26="One-time")*K22*Missions!$E$5:$E$26*'VIP Levels'!$E$8*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*K16*Missions!$E$5:$E$26*'VIP Levels'!$E$8*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26="One-time")*K23*Missions!$E$5:$E$26*'VIP Levels'!$E$9*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*K17*Missions!$E$5:$E$26*'VIP Levels'!$E$9*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30)),0)</f>
-        <v>386</v>
+        <v>371</v>
       </c>
       <c r="L11" s="8">
         <f>ROUND(L19*'VIP Levels'!$B$16*'VIP Levels'!$E$5*(Inputs!$B$14-1)*('VIP Levels'!$D$16/30)+L20*'VIP Levels'!$B$17*'VIP Levels'!$E$6*(Inputs!$B$14-1)*('VIP Levels'!$D$17/30)+L21*'VIP Levels'!$B$18*'VIP Levels'!$E$7*(Inputs!$B$14-1)*('VIP Levels'!$D$18/30)+L22*'VIP Levels'!$B$19*'VIP Levels'!$E$8*(Inputs!$B$14-1)*('VIP Levels'!$D$19/30)+L23*'VIP Levels'!$B$20*'VIP Levels'!$E$9*(Inputs!$B$14-1)*('VIP Levels'!$D$20/30)+L19*'VIP Levels'!$B$24*'VIP Levels'!$E$5*(Inputs!$B$14-1)*('VIP Levels'!$D$24/30)+L20*'VIP Levels'!$B$25*'VIP Levels'!$E$6*(Inputs!$B$14-1)*('VIP Levels'!$D$25/30)+L21*'VIP Levels'!$B$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*('VIP Levels'!$D$26/30)+L22*'VIP Levels'!$B$27*'VIP Levels'!$E$8*(Inputs!$B$14-1)*('VIP Levels'!$D$27/30)+L23*'VIP Levels'!$B$28*'VIP Levels'!$E$9*(Inputs!$B$14-1)*('VIP Levels'!$D$28/30)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26="One-time")*L19*Missions!$E$5:$E$26*'VIP Levels'!$E$5*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*L13*Missions!$E$5:$E$26*'VIP Levels'!$E$5*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26="One-time")*L20*Missions!$E$5:$E$26*'VIP Levels'!$E$6*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*L14*Missions!$E$5:$E$26*'VIP Levels'!$E$6*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26="One-time")*L21*Missions!$E$5:$E$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*L15*Missions!$E$5:$E$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26="One-time")*L22*Missions!$E$5:$E$26*'VIP Levels'!$E$8*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*L16*Missions!$E$5:$E$26*'VIP Levels'!$E$8*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26="One-time")*L23*Missions!$E$5:$E$26*'VIP Levels'!$E$9*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*L17*Missions!$E$5:$E$26*'VIP Levels'!$E$9*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26="One-time")*L19*Missions!$E$5:$E$26*'VIP Levels'!$E$5*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*L13*Missions!$E$5:$E$26*'VIP Levels'!$E$5*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26="One-time")*L20*Missions!$E$5:$E$26*'VIP Levels'!$E$6*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*L14*Missions!$E$5:$E$26*'VIP Levels'!$E$6*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26="One-time")*L21*Missions!$E$5:$E$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*L15*Missions!$E$5:$E$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26="One-time")*L22*Missions!$E$5:$E$26*'VIP Levels'!$E$8*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*L16*Missions!$E$5:$E$26*'VIP Levels'!$E$8*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26="One-time")*L23*Missions!$E$5:$E$26*'VIP Levels'!$E$9*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*L17*Missions!$E$5:$E$26*'VIP Levels'!$E$9*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30)),0)</f>
-        <v>451</v>
+        <v>432</v>
       </c>
       <c r="M11" s="8">
         <f>ROUND(M19*'VIP Levels'!$B$16*'VIP Levels'!$E$5*(Inputs!$B$14-1)*('VIP Levels'!$D$16/30)+M20*'VIP Levels'!$B$17*'VIP Levels'!$E$6*(Inputs!$B$14-1)*('VIP Levels'!$D$17/30)+M21*'VIP Levels'!$B$18*'VIP Levels'!$E$7*(Inputs!$B$14-1)*('VIP Levels'!$D$18/30)+M22*'VIP Levels'!$B$19*'VIP Levels'!$E$8*(Inputs!$B$14-1)*('VIP Levels'!$D$19/30)+M23*'VIP Levels'!$B$20*'VIP Levels'!$E$9*(Inputs!$B$14-1)*('VIP Levels'!$D$20/30)+M19*'VIP Levels'!$B$24*'VIP Levels'!$E$5*(Inputs!$B$14-1)*('VIP Levels'!$D$24/30)+M20*'VIP Levels'!$B$25*'VIP Levels'!$E$6*(Inputs!$B$14-1)*('VIP Levels'!$D$25/30)+M21*'VIP Levels'!$B$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*('VIP Levels'!$D$26/30)+M22*'VIP Levels'!$B$27*'VIP Levels'!$E$8*(Inputs!$B$14-1)*('VIP Levels'!$D$27/30)+M23*'VIP Levels'!$B$28*'VIP Levels'!$E$9*(Inputs!$B$14-1)*('VIP Levels'!$D$28/30)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26="One-time")*M19*Missions!$E$5:$E$26*'VIP Levels'!$E$5*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*M13*Missions!$E$5:$E$26*'VIP Levels'!$E$5*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26="One-time")*M20*Missions!$E$5:$E$26*'VIP Levels'!$E$6*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*M14*Missions!$E$5:$E$26*'VIP Levels'!$E$6*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26="One-time")*M21*Missions!$E$5:$E$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*M15*Missions!$E$5:$E$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26="One-time")*M22*Missions!$E$5:$E$26*'VIP Levels'!$E$8*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*M16*Missions!$E$5:$E$26*'VIP Levels'!$E$8*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26="One-time")*M23*Missions!$E$5:$E$26*'VIP Levels'!$E$9*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*M17*Missions!$E$5:$E$26*'VIP Levels'!$E$9*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26="One-time")*M19*Missions!$E$5:$E$26*'VIP Levels'!$E$5*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*M13*Missions!$E$5:$E$26*'VIP Levels'!$E$5*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26="One-time")*M20*Missions!$E$5:$E$26*'VIP Levels'!$E$6*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*M14*Missions!$E$5:$E$26*'VIP Levels'!$E$6*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26="One-time")*M21*Missions!$E$5:$E$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*M15*Missions!$E$5:$E$26*'VIP Levels'!$E$7*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26="One-time")*M22*Missions!$E$5:$E$26*'VIP Levels'!$E$8*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*M16*Missions!$E$5:$E$26*'VIP Levels'!$E$8*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26="One-time")*M23*Missions!$E$5:$E$26*'VIP Levels'!$E$9*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30))+SUMPRODUCT((Missions!$F$5:$F$26="Discount")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*M17*Missions!$E$5:$E$26*'VIP Levels'!$E$9*(Inputs!$B$14-1)*(Missions!$H$5:$H$26/30)),0)</f>
-        <v>523</v>
+        <v>501</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -7898,47 +7898,47 @@
       </c>
       <c r="C4" s="8">
         <f>'Affiliate Projection'!C9</f>
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D4" s="8">
         <f>'Affiliate Projection'!D9</f>
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="E4" s="8">
         <f>'Affiliate Projection'!E9</f>
-        <v>1407</v>
+        <v>1405</v>
       </c>
       <c r="F4" s="8">
         <f>'Affiliate Projection'!F9</f>
-        <v>1969</v>
+        <v>1965</v>
       </c>
       <c r="G4" s="8">
         <f>'Affiliate Projection'!G9</f>
-        <v>2597</v>
+        <v>2591</v>
       </c>
       <c r="H4" s="8">
         <f>'Affiliate Projection'!H9</f>
-        <v>3377</v>
+        <v>3369</v>
       </c>
       <c r="I4" s="8">
         <f>'Affiliate Projection'!I9</f>
-        <v>4255</v>
+        <v>4245</v>
       </c>
       <c r="J4" s="8">
         <f>'Affiliate Projection'!J9</f>
-        <v>5154</v>
+        <v>5142</v>
       </c>
       <c r="K4" s="8">
         <f>'Affiliate Projection'!K9</f>
-        <v>6178</v>
+        <v>6163</v>
       </c>
       <c r="L4" s="8">
         <f>'Affiliate Projection'!L9</f>
-        <v>7301</v>
+        <v>7282</v>
       </c>
       <c r="M4" s="8">
         <f>'Affiliate Projection'!M9</f>
-        <v>8533</v>
+        <v>8511</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -8004,47 +8004,47 @@
       </c>
       <c r="C6" s="10">
         <f t="shared" si="0"/>
-        <v>32874.520000000004</v>
+        <v>32814.53</v>
       </c>
       <c r="D6" s="10">
         <f t="shared" si="0"/>
-        <v>54050.990000000005</v>
+        <v>53991</v>
       </c>
       <c r="E6" s="10">
         <f t="shared" si="0"/>
-        <v>84405.930000000008</v>
+        <v>84285.95</v>
       </c>
       <c r="F6" s="10">
         <f t="shared" si="0"/>
-        <v>118120.31</v>
+        <v>117880.35</v>
       </c>
       <c r="G6" s="10">
         <f t="shared" si="0"/>
-        <v>155794.03</v>
+        <v>155434.09</v>
       </c>
       <c r="H6" s="10">
         <f t="shared" si="0"/>
-        <v>202586.23</v>
+        <v>202106.31</v>
       </c>
       <c r="I6" s="10">
         <f t="shared" si="0"/>
-        <v>255257.45</v>
+        <v>254657.55000000002</v>
       </c>
       <c r="J6" s="10">
         <f t="shared" si="0"/>
-        <v>309188.46000000002</v>
+        <v>308468.58</v>
       </c>
       <c r="K6" s="10">
         <f t="shared" si="0"/>
-        <v>370618.22000000003</v>
+        <v>369718.37</v>
       </c>
       <c r="L6" s="10">
         <f t="shared" si="0"/>
-        <v>437986.99</v>
+        <v>436847.18</v>
       </c>
       <c r="M6" s="10">
         <f t="shared" si="0"/>
-        <v>511894.67000000004</v>
+        <v>510574.89</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -8110,47 +8110,47 @@
       </c>
       <c r="C8" s="10">
         <f t="shared" si="2"/>
-        <v>31048.157777777778</v>
+        <v>30991.500555555558</v>
       </c>
       <c r="D8" s="10">
         <f t="shared" si="2"/>
-        <v>51048.157222222224</v>
+        <v>50991.5</v>
       </c>
       <c r="E8" s="10">
         <f t="shared" si="2"/>
-        <v>79716.71166666667</v>
+        <v>79603.397222222222</v>
       </c>
       <c r="F8" s="10">
         <f t="shared" si="2"/>
-        <v>111558.07055555556</v>
+        <v>111331.44166666667</v>
       </c>
       <c r="G8" s="10">
         <f t="shared" si="2"/>
-        <v>147138.8061111111</v>
+        <v>146798.86277777777</v>
       </c>
       <c r="H8" s="10">
         <f t="shared" si="2"/>
-        <v>191331.43944444446</v>
+        <v>190878.18166666667</v>
       </c>
       <c r="I8" s="10">
         <f t="shared" si="2"/>
-        <v>241076.48055555555</v>
+        <v>240509.90833333333</v>
       </c>
       <c r="J8" s="10">
         <f t="shared" si="2"/>
-        <v>292011.32333333336</v>
+        <v>291331.43666666665</v>
       </c>
       <c r="K8" s="10">
         <f t="shared" si="2"/>
-        <v>350028.31888888893</v>
+        <v>349178.46055555559</v>
       </c>
       <c r="L8" s="10">
         <f t="shared" si="2"/>
-        <v>413654.37944444444</v>
+        <v>412577.89222222223</v>
       </c>
       <c r="M8" s="10">
         <f t="shared" si="2"/>
-        <v>483456.07722222223</v>
+        <v>482209.61833333335</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.35">
@@ -8232,7 +8232,7 @@
   <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8316,47 +8316,47 @@
       </c>
       <c r="C5" s="10">
         <f>Revenue!C8*SUMPRODUCT('VIP Levels'!$D$5:$D$9,Inputs!C$23:C$27)</f>
-        <v>6209.6315555555557</v>
+        <v>6198.3001111111116</v>
       </c>
       <c r="D5" s="10">
         <f>Revenue!D8*SUMPRODUCT('VIP Levels'!$D$5:$D$9,Inputs!D$23:D$27)</f>
-        <v>10209.631444444445</v>
+        <v>10198.300000000001</v>
       </c>
       <c r="E5" s="10">
         <f>Revenue!E8*SUMPRODUCT('VIP Levels'!$D$5:$D$9,Inputs!E$23:E$27)</f>
-        <v>15943.342333333338</v>
+        <v>15920.679444444448</v>
       </c>
       <c r="F5" s="10">
         <f>Revenue!F8*SUMPRODUCT('VIP Levels'!$D$5:$D$9,Inputs!F$23:F$27)</f>
-        <v>22311.61411111111</v>
+        <v>22266.28833333333</v>
       </c>
       <c r="G5" s="10">
         <f>Revenue!G8*SUMPRODUCT('VIP Levels'!$D$5:$D$9,Inputs!G$23:G$27)</f>
-        <v>29427.761222222227</v>
+        <v>29359.772555555559</v>
       </c>
       <c r="H5" s="10">
         <f>Revenue!H8*SUMPRODUCT('VIP Levels'!$D$5:$D$9,Inputs!H$23:H$27)</f>
-        <v>38266.287888888903</v>
+        <v>38175.636333333343</v>
       </c>
       <c r="I5" s="10">
         <f>Revenue!I8*SUMPRODUCT('VIP Levels'!$D$5:$D$9,Inputs!I$23:I$27)</f>
-        <v>48215.296111111114</v>
+        <v>48101.981666666667</v>
       </c>
       <c r="J5" s="10">
         <f>Revenue!J8*SUMPRODUCT('VIP Levels'!$D$5:$D$9,Inputs!J$23:J$27)</f>
-        <v>58402.264666666684</v>
+        <v>58266.287333333341</v>
       </c>
       <c r="K5" s="10">
         <f>Revenue!K8*SUMPRODUCT('VIP Levels'!$D$5:$D$9,Inputs!K$23:K$27)</f>
-        <v>70005.663777777794</v>
+        <v>69835.692111111115</v>
       </c>
       <c r="L5" s="10">
         <f>Revenue!L8*SUMPRODUCT('VIP Levels'!$D$5:$D$9,Inputs!L$23:L$27)</f>
-        <v>82730.875888888899</v>
+        <v>82515.578444444458</v>
       </c>
       <c r="M5" s="10">
         <f>Revenue!M8*SUMPRODUCT('VIP Levels'!$D$5:$D$9,Inputs!M$23:M$27)</f>
-        <v>96691.215444444446</v>
+        <v>96441.923666666669</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -8422,47 +8422,47 @@
       </c>
       <c r="C7" s="10">
         <f>SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!C19*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!C13*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!C20*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!C14*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!C21*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!C15*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!C22*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!C16*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!C23*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!C17*Missions!$E$5:$E$26*Missions!$J$5:$J$26)</f>
-        <v>309.34843333333339</v>
+        <v>296.97449600000004</v>
       </c>
       <c r="D7" s="10">
         <f>SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!D19*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!D13*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!D20*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!D14*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!D21*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!D15*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!D22*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!D16*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!D23*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!D17*Missions!$E$5:$E$26*Missions!$J$5:$J$26)</f>
-        <v>779.55805200000009</v>
+        <v>754.8101773333334</v>
       </c>
       <c r="E7" s="10">
         <f>SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!E19*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!E13*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!E20*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!E14*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!E21*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!E15*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!E22*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!E16*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!E23*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!E17*Missions!$E$5:$E$26*Missions!$J$5:$J$26)</f>
-        <v>1525.0877763333333</v>
+        <v>1469.4050583333335</v>
       </c>
       <c r="F7" s="10">
         <f>SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!F19*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!F13*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!F20*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!F14*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!F21*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!F15*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!F22*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!F16*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!F23*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!F17*Missions!$E$5:$E$26*Missions!$J$5:$J$26)</f>
-        <v>2462.4135293333338</v>
+        <v>2375.7959680000004</v>
       </c>
       <c r="G7" s="10">
         <f>SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!G19*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!G13*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!G20*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!G14*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!G21*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!G15*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!G22*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!G16*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!G23*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!G17*Missions!$E$5:$E$26*Missions!$J$5:$J$26)</f>
-        <v>3486.3568436666674</v>
+        <v>3356.4305016666676</v>
       </c>
       <c r="H7" s="10">
         <f>SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!H19*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!H13*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!H20*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!H14*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!H21*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!H15*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!H22*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!H16*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!H23*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!H17*Missions!$E$5:$E$26*Missions!$J$5:$J$26)</f>
-        <v>4890.7987310000008</v>
+        <v>4711.3766396666679</v>
       </c>
       <c r="I7" s="10">
         <f>SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!I19*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!I13*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!I20*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!I14*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!I21*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!I15*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!I22*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!I16*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!I23*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!I17*Missions!$E$5:$E$26*Missions!$J$5:$J$26)</f>
-        <v>6527.2519433333346</v>
+        <v>6292.1471340000007</v>
       </c>
       <c r="J7" s="10">
         <f>SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!J19*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!J13*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!J20*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!J14*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!J21*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!J15*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!J22*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!J16*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!J23*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!J17*Missions!$E$5:$E$26*Missions!$J$5:$J$26)</f>
-        <v>8210.1074206666672</v>
+        <v>7913.1329246666673</v>
       </c>
       <c r="K7" s="10">
         <f>SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!K19*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!K13*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!K20*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!K14*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!K21*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!K15*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!K22*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!K16*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!K23*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!K17*Missions!$E$5:$E$26*Missions!$J$5:$J$26)</f>
-        <v>10140.441644666669</v>
+        <v>9769.2235246666678</v>
       </c>
       <c r="L7" s="10">
         <f>SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!L19*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!L13*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!L20*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!L14*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!L21*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!L15*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!L22*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!L16*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!L23*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!L17*Missions!$E$5:$E$26*Missions!$J$5:$J$26)</f>
-        <v>12296.600225000002</v>
+        <v>11844.951512333335</v>
       </c>
       <c r="M7" s="10">
         <f>SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!M19*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Bronze")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!M13*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!M20*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Silver")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!M14*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!M21*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Gold")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!M15*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!M22*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Platinum")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!M16*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26="One-time")*'Affiliate Projection'!M23*Missions!$E$5:$E$26*Missions!$J$5:$J$26)+SUMPRODUCT((Missions!$F$5:$F$26="Commission Boost")*(Missions!$A$5:$A$26="Diamond")*(Missions!$D$5:$D$26&lt;&gt;"One-time")*'Affiliate Projection'!M17*Missions!$E$5:$E$26*Missions!$J$5:$J$26)</f>
-        <v>14694.050583333334</v>
+        <v>14149.597340666667</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -8581,47 +8581,47 @@
       </c>
       <c r="C10" s="11">
         <f t="shared" si="0"/>
-        <v>8402.2360605555568</v>
+        <v>8378.530678777779</v>
       </c>
       <c r="D10" s="11">
         <f t="shared" si="0"/>
-        <v>13678.857143777779</v>
+        <v>13642.777824666668</v>
       </c>
       <c r="E10" s="11">
         <f t="shared" si="0"/>
-        <v>21611.333510666671</v>
+        <v>21532.987903777779</v>
       </c>
       <c r="F10" s="11">
         <f t="shared" si="0"/>
-        <v>30011.582569111109</v>
+        <v>29879.639229999993</v>
       </c>
       <c r="G10" s="11">
         <f t="shared" si="0"/>
-        <v>39226.801776555563</v>
+        <v>39028.8867678889</v>
       </c>
       <c r="H10" s="11">
         <f t="shared" si="0"/>
-        <v>51408.579141888906</v>
+        <v>51138.505495000012</v>
       </c>
       <c r="I10" s="11">
         <f t="shared" si="0"/>
-        <v>64716.591436777788</v>
+        <v>64368.172183000002</v>
       </c>
       <c r="J10" s="11">
         <f t="shared" si="0"/>
-        <v>77845.957511000015</v>
+        <v>77413.005681666677</v>
       </c>
       <c r="K10" s="11">
         <f t="shared" si="0"/>
-        <v>93404.675292444459</v>
+        <v>92863.485505777775</v>
       </c>
       <c r="L10" s="11">
         <f t="shared" si="0"/>
-        <v>110316.54151155557</v>
+        <v>109649.59535444446</v>
       </c>
       <c r="M10" s="11">
         <f t="shared" si="0"/>
-        <v>128962.34002711112</v>
+        <v>128168.59500666667</v>
       </c>
       <c r="O10" s="66"/>
     </row>
@@ -8866,47 +8866,47 @@
       </c>
       <c r="C21" s="11">
         <f t="shared" si="3"/>
-        <v>10774.986060555557</v>
+        <v>10751.280678777779</v>
       </c>
       <c r="D21" s="11">
         <f t="shared" si="3"/>
-        <v>16713.607143777779</v>
+        <v>16677.527824666668</v>
       </c>
       <c r="E21" s="11">
         <f t="shared" si="3"/>
-        <v>25863.833510666671</v>
+        <v>25785.487903777779</v>
       </c>
       <c r="F21" s="11">
         <f t="shared" si="3"/>
-        <v>35083.582569111109</v>
+        <v>34951.639229999993</v>
       </c>
       <c r="G21" s="11">
         <f t="shared" si="3"/>
-        <v>45226.801776555563</v>
+        <v>45028.8867678889</v>
       </c>
       <c r="H21" s="11">
         <f t="shared" si="3"/>
-        <v>58785.579141888906</v>
+        <v>58515.505495000012</v>
       </c>
       <c r="I21" s="11">
         <f t="shared" si="3"/>
-        <v>73399.341436777788</v>
+        <v>73050.922183000002</v>
       </c>
       <c r="J21" s="11">
         <f t="shared" si="3"/>
-        <v>87415.957511000015</v>
+        <v>86983.005681666677</v>
       </c>
       <c r="K21" s="11">
         <f t="shared" si="3"/>
-        <v>104449.67529244446</v>
+        <v>103908.48550577777</v>
       </c>
       <c r="L21" s="11">
         <f t="shared" si="3"/>
-        <v>122810.79151155557</v>
+        <v>122143.84535444446</v>
       </c>
       <c r="M21" s="11">
         <f t="shared" si="3"/>
-        <v>143039.09002711112</v>
+        <v>142245.34500666667</v>
       </c>
       <c r="O21" s="66"/>
     </row>
@@ -9378,47 +9378,47 @@
       </c>
       <c r="C5" s="201">
         <f>'Affiliate Projection'!C9</f>
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D5" s="201">
         <f>'Affiliate Projection'!D9</f>
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="E5" s="201">
         <f>'Affiliate Projection'!E9</f>
-        <v>1407</v>
+        <v>1405</v>
       </c>
       <c r="F5" s="201">
         <f>'Affiliate Projection'!F9</f>
-        <v>1969</v>
+        <v>1965</v>
       </c>
       <c r="G5" s="201">
         <f>'Affiliate Projection'!G9</f>
-        <v>2597</v>
+        <v>2591</v>
       </c>
       <c r="H5" s="201">
         <f>'Affiliate Projection'!H9</f>
-        <v>3377</v>
+        <v>3369</v>
       </c>
       <c r="I5" s="201">
         <f>'Affiliate Projection'!I9</f>
-        <v>4255</v>
+        <v>4245</v>
       </c>
       <c r="J5" s="201">
         <f>'Affiliate Projection'!J9</f>
-        <v>5154</v>
+        <v>5142</v>
       </c>
       <c r="K5" s="201">
         <f>'Affiliate Projection'!K9</f>
-        <v>6178</v>
+        <v>6163</v>
       </c>
       <c r="L5" s="201">
         <f>'Affiliate Projection'!L9</f>
-        <v>7301</v>
+        <v>7282</v>
       </c>
       <c r="M5" s="201">
         <f>'Affiliate Projection'!M9</f>
-        <v>8533</v>
+        <v>8511</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -9431,47 +9431,47 @@
       </c>
       <c r="C6" s="202">
         <f>Revenue!C8</f>
-        <v>31048.157777777778</v>
+        <v>30991.500555555558</v>
       </c>
       <c r="D6" s="202">
         <f>Revenue!D8</f>
-        <v>51048.157222222224</v>
+        <v>50991.5</v>
       </c>
       <c r="E6" s="202">
         <f>Revenue!E8</f>
-        <v>79716.71166666667</v>
+        <v>79603.397222222222</v>
       </c>
       <c r="F6" s="202">
         <f>Revenue!F8</f>
-        <v>111558.07055555556</v>
+        <v>111331.44166666667</v>
       </c>
       <c r="G6" s="202">
         <f>Revenue!G8</f>
-        <v>147138.8061111111</v>
+        <v>146798.86277777777</v>
       </c>
       <c r="H6" s="202">
         <f>Revenue!H8</f>
-        <v>191331.43944444446</v>
+        <v>190878.18166666667</v>
       </c>
       <c r="I6" s="202">
         <f>Revenue!I8</f>
-        <v>241076.48055555555</v>
+        <v>240509.90833333333</v>
       </c>
       <c r="J6" s="202">
         <f>Revenue!J8</f>
-        <v>292011.32333333336</v>
+        <v>291331.43666666665</v>
       </c>
       <c r="K6" s="202">
         <f>Revenue!K8</f>
-        <v>350028.31888888893</v>
+        <v>349178.46055555559</v>
       </c>
       <c r="L6" s="202">
         <f>Revenue!L8</f>
-        <v>413654.37944444444</v>
+        <v>412577.89222222223</v>
       </c>
       <c r="M6" s="202">
         <f>Revenue!M8</f>
-        <v>483456.07722222223</v>
+        <v>482209.61833333335</v>
       </c>
       <c r="N6" s="66"/>
     </row>
@@ -9485,47 +9485,47 @@
       </c>
       <c r="C7" s="204">
         <f t="shared" ref="C7:L7" si="0">SUM(C10:C13)+SUM(C18:C19)+C24</f>
-        <v>10774.986060555557</v>
+        <v>10751.280678777779</v>
       </c>
       <c r="D7" s="204">
         <f t="shared" si="0"/>
-        <v>16713.607143777779</v>
+        <v>16677.527824666668</v>
       </c>
       <c r="E7" s="204">
         <f t="shared" si="0"/>
-        <v>25863.833510666671</v>
+        <v>25785.487903777779</v>
       </c>
       <c r="F7" s="204">
         <f t="shared" si="0"/>
-        <v>35083.582569111109</v>
+        <v>34951.639230000001</v>
       </c>
       <c r="G7" s="204">
         <f t="shared" si="0"/>
-        <v>45226.801776555563</v>
+        <v>45028.886767888893</v>
       </c>
       <c r="H7" s="204">
         <f t="shared" si="0"/>
-        <v>58785.579141888906</v>
+        <v>58515.505495000012</v>
       </c>
       <c r="I7" s="204">
         <f t="shared" si="0"/>
-        <v>73399.341436777788</v>
+        <v>73050.922183000002</v>
       </c>
       <c r="J7" s="204">
         <f t="shared" si="0"/>
-        <v>87415.957511000015</v>
+        <v>86983.005681666677</v>
       </c>
       <c r="K7" s="204">
         <f t="shared" si="0"/>
-        <v>104449.67529244447</v>
+        <v>103908.48550577779</v>
       </c>
       <c r="L7" s="204">
         <f t="shared" si="0"/>
-        <v>122810.79151155557</v>
+        <v>122143.84535444446</v>
       </c>
       <c r="M7" s="204">
         <f>SUM(M10:M13)+SUM(M18:M19)+M24</f>
-        <v>143039.09002711112</v>
+        <v>142245.34500666667</v>
       </c>
       <c r="N7" s="199"/>
     </row>
@@ -9604,47 +9604,47 @@
       </c>
       <c r="C11" s="69">
         <f>'Affiliate Costs'!C7</f>
-        <v>309.34843333333339</v>
+        <v>296.97449600000004</v>
       </c>
       <c r="D11" s="69">
         <f>'Affiliate Costs'!D7</f>
-        <v>779.55805200000009</v>
+        <v>754.8101773333334</v>
       </c>
       <c r="E11" s="69">
         <f>'Affiliate Costs'!E7</f>
-        <v>1525.0877763333333</v>
+        <v>1469.4050583333335</v>
       </c>
       <c r="F11" s="69">
         <f>'Affiliate Costs'!F7</f>
-        <v>2462.4135293333338</v>
+        <v>2375.7959680000004</v>
       </c>
       <c r="G11" s="69">
         <f>'Affiliate Costs'!G7</f>
-        <v>3486.3568436666674</v>
+        <v>3356.4305016666676</v>
       </c>
       <c r="H11" s="69">
         <f>'Affiliate Costs'!H7</f>
-        <v>4890.7987310000008</v>
+        <v>4711.3766396666679</v>
       </c>
       <c r="I11" s="69">
         <f>'Affiliate Costs'!I7</f>
-        <v>6527.2519433333346</v>
+        <v>6292.1471340000007</v>
       </c>
       <c r="J11" s="69">
         <f>'Affiliate Costs'!J7</f>
-        <v>8210.1074206666672</v>
+        <v>7913.1329246666673</v>
       </c>
       <c r="K11" s="69">
         <f>'Affiliate Costs'!K7</f>
-        <v>10140.441644666669</v>
+        <v>9769.2235246666678</v>
       </c>
       <c r="L11" s="69">
         <f>'Affiliate Costs'!L7</f>
-        <v>12296.600225000002</v>
+        <v>11844.951512333335</v>
       </c>
       <c r="M11" s="69">
         <f>'Affiliate Costs'!M7</f>
-        <v>14694.050583333334</v>
+        <v>14149.597340666667</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -9763,47 +9763,47 @@
       </c>
       <c r="C14" s="164">
         <f t="shared" si="1"/>
-        <v>5.720935994525548</v>
+        <v>5.7087732864107252</v>
       </c>
       <c r="D14" s="164">
         <f t="shared" si="1"/>
-        <v>5.0329056330003699</v>
+        <v>5.0110001118518523</v>
       </c>
       <c r="E14" s="164">
         <f t="shared" si="1"/>
-        <v>4.9590744643449423</v>
+        <v>4.9265018173190986</v>
       </c>
       <c r="F14" s="164">
         <f t="shared" si="1"/>
-        <v>4.5716652899949217</v>
+        <v>4.5368912949957592</v>
       </c>
       <c r="G14" s="164">
         <f t="shared" si="1"/>
-        <v>4.2892419446797589</v>
+        <v>4.249029327801364</v>
       </c>
       <c r="H14" s="164">
         <f t="shared" si="1"/>
-        <v>4.2883771575362752</v>
+        <v>4.2453035232017422</v>
       </c>
       <c r="I14" s="164">
         <f t="shared" si="1"/>
-        <v>4.1785672318840579</v>
+        <v>4.133026799136239</v>
       </c>
       <c r="J14" s="164">
         <f t="shared" si="1"/>
-        <v>3.9672357086405379</v>
+        <v>3.9187394683650978</v>
       </c>
       <c r="K14" s="164">
         <f t="shared" si="1"/>
-        <v>3.9270393209237082</v>
+        <v>3.8763639144356108</v>
       </c>
       <c r="L14" s="164">
         <f t="shared" si="1"/>
-        <v>3.864343196365795</v>
+        <v>3.8124033183191437</v>
       </c>
       <c r="M14" s="164">
         <f t="shared" si="1"/>
-        <v>3.8196956951443415</v>
+        <v>3.7655986516273057</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -9816,47 +9816,47 @@
       </c>
       <c r="C15" s="72">
         <f>C14/Inputs!$B$12</f>
-        <v>9.5364827379989123E-2</v>
+        <v>9.5162081787143277E-2</v>
       </c>
       <c r="D15" s="72">
         <f>D14/Inputs!$B$12</f>
-        <v>8.389574317386847E-2</v>
+        <v>8.3530590295913518E-2</v>
       </c>
       <c r="E15" s="72">
         <f>E14/Inputs!$B$12</f>
-        <v>8.2665018575511617E-2</v>
+        <v>8.2122050630423382E-2</v>
       </c>
       <c r="F15" s="72">
         <f>F14/Inputs!$B$12</f>
-        <v>7.6207122687029866E-2</v>
+        <v>7.5627459493178173E-2</v>
       </c>
       <c r="G15" s="72">
         <f>G14/Inputs!$B$12</f>
-        <v>7.1499282291711264E-2</v>
+        <v>7.0828960290071075E-2</v>
       </c>
       <c r="H15" s="72">
         <f>H14/Inputs!$B$12</f>
-        <v>7.1484866770066269E-2</v>
+        <v>7.0766853195561627E-2</v>
       </c>
       <c r="I15" s="72">
         <f>I14/Inputs!$B$12</f>
-        <v>6.9654396264111643E-2</v>
+        <v>6.8895262529358875E-2</v>
       </c>
       <c r="J15" s="72">
         <f>J14/Inputs!$B$12</f>
-        <v>6.6131617080188998E-2</v>
+        <v>6.5323211674697415E-2</v>
       </c>
       <c r="K15" s="72">
         <f>K14/Inputs!$B$12</f>
-        <v>6.5461565609663416E-2</v>
+        <v>6.461683471304569E-2</v>
       </c>
       <c r="L15" s="72">
         <f>L14/Inputs!$B$12</f>
-        <v>6.4416456015432486E-2</v>
+        <v>6.3550647079832365E-2</v>
       </c>
       <c r="M15" s="72">
         <f>M14/Inputs!$B$12</f>
-        <v>6.3672206953564611E-2</v>
+        <v>6.2770439266999586E-2</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -10018,47 +10018,47 @@
       </c>
       <c r="C20" s="164">
         <f t="shared" si="2"/>
-        <v>2.6100028832116795</v>
+        <v>2.6147743692870207</v>
       </c>
       <c r="D20" s="164">
         <f t="shared" si="2"/>
-        <v>2.1857133451720312</v>
+        <v>2.1881419155555557</v>
       </c>
       <c r="E20" s="164">
         <f t="shared" si="2"/>
-        <v>2.0917366069651746</v>
+        <v>2.0947141679715306</v>
       </c>
       <c r="F20" s="164">
         <f t="shared" si="2"/>
-        <v>1.9148600822752668</v>
+        <v>1.9187580162849873</v>
       </c>
       <c r="G20" s="164">
         <f t="shared" si="2"/>
-        <v>1.7943316226415096</v>
+        <v>1.7984867711308377</v>
       </c>
       <c r="H20" s="164">
         <f t="shared" si="2"/>
-        <v>1.7878121385845429</v>
+        <v>1.7920574627485903</v>
       </c>
       <c r="I20" s="164">
         <f t="shared" si="2"/>
-        <v>1.7401273217391307</v>
+        <v>1.7442265616018846</v>
       </c>
       <c r="J20" s="164">
         <f t="shared" si="2"/>
-        <v>1.6621187431121462</v>
+        <v>1.6659976666666672</v>
       </c>
       <c r="K20" s="164">
         <f t="shared" si="2"/>
-        <v>1.6482296196179997</v>
+        <v>1.6522412120720431</v>
       </c>
       <c r="L20" s="164">
         <f t="shared" si="2"/>
-        <v>1.6253041975071909</v>
+        <v>1.6295448978302667</v>
       </c>
       <c r="M20" s="164">
         <f t="shared" si="2"/>
-        <v>1.611908029532404</v>
+        <v>1.6160746347080253</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -10071,47 +10071,47 @@
       </c>
       <c r="C21" s="72">
         <f>C20/Inputs!$B$12</f>
-        <v>4.3507299270073005E-2</v>
+        <v>4.3586837294332735E-2</v>
       </c>
       <c r="D21" s="72">
         <f>D20/Inputs!$B$12</f>
-        <v>3.6434628190899002E-2</v>
+        <v>3.6475111111111111E-2</v>
       </c>
       <c r="E21" s="72">
         <f>E20/Inputs!$B$12</f>
-        <v>3.4868088130774702E-2</v>
+        <v>3.4917722419928833E-2</v>
       </c>
       <c r="F21" s="72">
         <f>F20/Inputs!$B$12</f>
-        <v>3.191965464702895E-2</v>
+        <v>3.1984631043256995E-2</v>
       </c>
       <c r="G21" s="72">
         <f>G20/Inputs!$B$12</f>
-        <v>2.9910512129380055E-2</v>
+        <v>2.9979776148205326E-2</v>
       </c>
       <c r="H21" s="72">
         <f>H20/Inputs!$B$12</f>
-        <v>2.9801835949067226E-2</v>
+        <v>2.9872603146334227E-2</v>
       </c>
       <c r="I21" s="72">
         <f>I20/Inputs!$B$12</f>
-        <v>2.9006956521739131E-2</v>
+        <v>2.9075288574793873E-2</v>
       </c>
       <c r="J21" s="72">
         <f>J20/Inputs!$B$12</f>
-        <v>2.7706596818005438E-2</v>
+        <v>2.7771256320497869E-2</v>
       </c>
       <c r="K21" s="72">
         <f>K20/Inputs!$B$12</f>
-        <v>2.7475072839106513E-2</v>
+        <v>2.754194385851047E-2</v>
       </c>
       <c r="L21" s="72">
         <f>L20/Inputs!$B$12</f>
-        <v>2.7092918778249556E-2</v>
+        <v>2.7163608898654219E-2</v>
       </c>
       <c r="M21" s="72">
         <f>M20/Inputs!$B$12</f>
-        <v>2.6869612094222436E-2</v>
+        <v>2.6939067089648695E-2</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -10129,47 +10129,47 @@
       </c>
       <c r="C24" s="69">
         <f>'Affiliate Costs'!C5</f>
-        <v>6209.6315555555557</v>
+        <v>6198.3001111111116</v>
       </c>
       <c r="D24" s="69">
         <f>'Affiliate Costs'!D5</f>
-        <v>10209.631444444445</v>
+        <v>10198.300000000001</v>
       </c>
       <c r="E24" s="69">
         <f>'Affiliate Costs'!E5</f>
-        <v>15943.342333333338</v>
+        <v>15920.679444444448</v>
       </c>
       <c r="F24" s="69">
         <f>'Affiliate Costs'!F5</f>
-        <v>22311.61411111111</v>
+        <v>22266.28833333333</v>
       </c>
       <c r="G24" s="69">
         <f>'Affiliate Costs'!G5</f>
-        <v>29427.761222222227</v>
+        <v>29359.772555555559</v>
       </c>
       <c r="H24" s="69">
         <f>'Affiliate Costs'!H5</f>
-        <v>38266.287888888903</v>
+        <v>38175.636333333343</v>
       </c>
       <c r="I24" s="69">
         <f>'Affiliate Costs'!I5</f>
-        <v>48215.296111111114</v>
+        <v>48101.981666666667</v>
       </c>
       <c r="J24" s="69">
         <f>'Affiliate Costs'!J5</f>
-        <v>58402.264666666684</v>
+        <v>58266.287333333341</v>
       </c>
       <c r="K24" s="69">
         <f>'Affiliate Costs'!K5</f>
-        <v>70005.663777777794</v>
+        <v>69835.692111111115</v>
       </c>
       <c r="L24" s="69">
         <f>'Affiliate Costs'!L5</f>
-        <v>82730.875888888899</v>
+        <v>82515.578444444458</v>
       </c>
       <c r="M24" s="69">
         <f>'Affiliate Costs'!M5</f>
-        <v>96691.215444444446</v>
+        <v>96441.923666666669</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -10198,11 +10198,11 @@
       </c>
       <c r="G25" s="164">
         <f t="shared" si="3"/>
-        <v>11.331444444444447</v>
+        <v>11.331444444444445</v>
       </c>
       <c r="H25" s="164">
         <f t="shared" si="3"/>
-        <v>11.331444444444449</v>
+        <v>11.331444444444447</v>
       </c>
       <c r="I25" s="164">
         <f t="shared" si="3"/>
@@ -10210,15 +10210,15 @@
       </c>
       <c r="J25" s="164">
         <f t="shared" si="3"/>
-        <v>11.331444444444449</v>
+        <v>11.331444444444445</v>
       </c>
       <c r="K25" s="164">
         <f t="shared" si="3"/>
-        <v>11.331444444444447</v>
+        <v>11.331444444444445</v>
       </c>
       <c r="L25" s="164">
         <f t="shared" si="3"/>
-        <v>11.331444444444445</v>
+        <v>11.331444444444447</v>
       </c>
       <c r="M25" s="164">
         <f t="shared" si="3"/>
@@ -10255,7 +10255,7 @@
       </c>
       <c r="H26" s="72">
         <f t="shared" si="4"/>
-        <v>0.20000000000000007</v>
+        <v>0.20000000000000004</v>
       </c>
       <c r="I26" s="72">
         <f t="shared" si="4"/>
@@ -10267,7 +10267,7 @@
       </c>
       <c r="K26" s="72">
         <f t="shared" si="4"/>
-        <v>0.2</v>
+        <v>0.19999999999999998</v>
       </c>
       <c r="L26" s="72">
         <f t="shared" si="4"/>
@@ -10300,7 +10300,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:T82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A26" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="L70" sqref="L70"/>
     </sheetView>
   </sheetViews>

</xml_diff>